<commit_message>
generic commit message, Tue 22:52:42 12.09.2023.
</commit_message>
<xml_diff>
--- a/dataset05-scaling_babb02,babb03.xlsx
+++ b/dataset05-scaling_babb02,babb03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74568E39-AA89-4A82-9830-196503F372A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F4F31C-6EB4-47BD-8B39-6C603F9B2C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9330" yWindow="0" windowWidth="19470" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -161,18 +161,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,32 +519,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <f>1/C2</f>
         <v>1.1764705882352942</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <f>1/D2</f>
         <v>1.1764705882352942</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <f>1/E2</f>
         <v>0.1</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="8">
+      <c r="F3" s="8"/>
+      <c r="G3" s="7">
         <f>1/G2</f>
         <v>1</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <f>1/H2</f>
         <v>1</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <f>1/I2</f>
         <v>1</v>
       </c>
@@ -556,15 +554,15 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <f>C6/C2</f>
+        <f t="shared" ref="C4:E5" si="0">C6/C2</f>
         <v>2.9764705882352938</v>
       </c>
       <c r="D4">
-        <f>D6/D2</f>
+        <f t="shared" si="0"/>
         <v>2.9764705882352938</v>
       </c>
       <c r="E4">
-        <f>E6/E2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4">
@@ -580,23 +578,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <f>C7/C3</f>
+        <f t="shared" si="0"/>
         <v>0.33596837944664032</v>
       </c>
       <c r="D5" s="1">
-        <f>D7/D3</f>
+        <f t="shared" si="0"/>
         <v>0.33596837944664032</v>
       </c>
       <c r="E5" s="1">
-        <f>E7/E3</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="9"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="8"/>
       <c r="G5" s="1">
         <f>C7/G3</f>
         <v>0.39525691699604748</v>
@@ -623,11 +621,9 @@
       <c r="E6">
         <v>10</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1">
@@ -642,10 +638,7 @@
         <f>1/E6</f>
         <v>0.1</v>
       </c>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G8" s="10"/>
+      <c r="F7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cropping coordinate tables Zusammentrag (partial)
</commit_message>
<xml_diff>
--- a/dataset05-scaling_babb02,babb03.xlsx
+++ b/dataset05-scaling_babb02,babb03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\imageProcessTif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F4F31C-6EB4-47BD-8B39-6C603F9B2C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B377423-3807-4AEA-A643-18AF0AE6715F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9330" yWindow="0" windowWidth="19470" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -454,16 +454,16 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>

</xml_diff>